<commit_message>
remove double conditionals so it works with the subset changes in the other repo
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Death.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Death.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/work/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDFEFAC3-E17B-9848-8ED2-FEF6D4BF194C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBDC7842-0A3A-714C-9128-63CE019AB624}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34400" yWindow="460" windowWidth="34400" windowHeight="28340" tabRatio="500" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17200" yWindow="460" windowWidth="34400" windowHeight="28340" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="notify_type_lookup" sheetId="11" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="70">
   <si>
     <t>casrec_code</t>
   </si>
@@ -169,24 +169,12 @@
     <t>PAT</t>
   </si>
   <si>
-    <t>conditional_lookup</t>
-  </si>
-  <si>
-    <t>letter_sent_death_lookup</t>
-  </si>
-  <si>
-    <t>Term Type</t>
-  </si>
-  <si>
     <t>datedeathcertificatereceived</t>
   </si>
   <si>
     <t>datenotified</t>
   </si>
   <si>
-    <t>notified_lookup</t>
-  </si>
-  <si>
     <t>notifiedby</t>
   </si>
   <si>
@@ -208,12 +196,6 @@
     <t>Deputy</t>
   </si>
   <si>
-    <t>deputy_date_of_death_lookup</t>
-  </si>
-  <si>
-    <t>Stat</t>
-  </si>
-  <si>
     <t>OTHER</t>
   </si>
   <si>
@@ -232,10 +214,6 @@
     <t>NO</t>
   </si>
   <si>
-    <t>proof_lookup
-proof_boolean_lookup</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -248,14 +226,6 @@
     <t>Death of client no</t>
   </si>
   <si>
-    <t>notify_lookup
-notify_type_lookup</t>
-  </si>
-  <si>
-    <t>termby_lookup
-termby_type_lookup</t>
-  </si>
-  <si>
     <t>Letter</t>
   </si>
   <si>
@@ -281,6 +251,12 @@
   </si>
   <si>
     <t>deputy</t>
+  </si>
+  <si>
+    <t>notify_type_lookup</t>
+  </si>
+  <si>
+    <t>proof_boolean_lookup</t>
   </si>
 </sst>
 </file>
@@ -301,26 +277,26 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -820,7 +796,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -852,7 +828,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="2"/>
@@ -884,7 +860,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="2"/>
@@ -916,7 +892,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="2"/>
@@ -948,7 +924,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="2"/>
@@ -979,7 +955,7 @@
         <v>5</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="2"/>
@@ -1010,7 +986,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -1073,7 +1049,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="O5" sqref="O5"/>
+      <selection pane="bottomLeft" activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -1245,22 +1221,16 @@
         <v>0</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="L5" s="13" t="s">
         <v>53</v>
       </c>
+      <c r="K5" s="5"/>
+      <c r="L5" s="13"/>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
-      <c r="O5" s="5" t="s">
-        <v>54</v>
-      </c>
+      <c r="O5" s="5"/>
       <c r="P5" s="6" t="s">
         <v>36</v>
       </c>
@@ -1273,7 +1243,7 @@
         <v>28</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>38</v>
@@ -1283,22 +1253,16 @@
         <v>0</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="L6" s="14" t="s">
         <v>53</v>
       </c>
+      <c r="K6" s="5"/>
+      <c r="L6" s="14"/>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
-      <c r="O6" s="5" t="s">
-        <v>54</v>
-      </c>
+      <c r="O6" s="5"/>
       <c r="P6" s="6" t="s">
         <v>36</v>
       </c>
@@ -1311,7 +1275,7 @@
         <v>28</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>38</v>
@@ -1321,22 +1285,16 @@
         <v>0</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="L7" s="14" t="s">
         <v>53</v>
       </c>
+      <c r="K7" s="5"/>
+      <c r="L7" s="14"/>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
-      <c r="O7" s="5" t="s">
-        <v>54</v>
-      </c>
+      <c r="O7" s="5"/>
       <c r="P7" s="6" t="s">
         <v>36</v>
       </c>
@@ -1349,10 +1307,10 @@
         <v>28</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E8" s="4" t="b">
         <f>FALSE()</f>
@@ -1363,12 +1321,10 @@
       <c r="K8" s="5"/>
       <c r="L8" s="14"/>
       <c r="M8" s="5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="N8" s="5"/>
-      <c r="O8" s="5" t="s">
-        <v>54</v>
-      </c>
+      <c r="O8" s="5"/>
       <c r="P8" s="6" t="s">
         <v>36</v>
       </c>
@@ -1381,10 +1337,10 @@
         <v>28</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E9" s="4" t="b">
         <f>FALSE()</f>
@@ -1395,7 +1351,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="12"/>
       <c r="M9" s="5" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
@@ -1411,10 +1367,10 @@
         <v>28</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E10" s="4" t="b">
         <f>FALSE()</f>
@@ -1425,12 +1381,10 @@
       <c r="K10" s="5"/>
       <c r="L10" s="14"/>
       <c r="M10" s="5" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="N10" s="5"/>
-      <c r="O10" s="5" t="s">
-        <v>42</v>
-      </c>
+      <c r="O10" s="5"/>
       <c r="P10" s="6" t="s">
         <v>36</v>
       </c>
@@ -1443,10 +1397,10 @@
         <v>28</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E11" s="4" t="b">
         <f>FALSE()</f>
@@ -1457,7 +1411,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="12"/>
       <c r="M11" s="5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
@@ -1525,10 +1479,10 @@
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -1784,11 +1738,11 @@
     </row>
     <row r="2" spans="1:24" ht="15">
       <c r="A2" s="4" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="5" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D2" s="5" t="b">
         <v>1</v>
@@ -1816,11 +1770,11 @@
     </row>
     <row r="3" spans="1:24" ht="15">
       <c r="A3" s="4" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D3" s="6" t="b">
         <v>0</v>
@@ -2570,14 +2524,14 @@
     </row>
     <row r="2" spans="1:24" ht="15">
       <c r="A2" s="4" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="5" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -2602,14 +2556,14 @@
     </row>
     <row r="3" spans="1:24" ht="15">
       <c r="A3" s="4" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="2"/>
@@ -2634,14 +2588,14 @@
     </row>
     <row r="4" spans="1:24" ht="15">
       <c r="A4" s="4" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="5" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="2"/>
@@ -2842,11 +2796,11 @@
     </row>
     <row r="2" spans="1:24" ht="15">
       <c r="A2" s="4" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="5" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>7</v>
@@ -3575,7 +3529,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P4" sqref="P4"/>
+      <selection pane="bottomLeft" activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -3698,7 +3652,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="32">
+    <row r="4" spans="1:17" ht="16">
       <c r="A4" s="4" t="s">
         <v>27</v>
       </c>
@@ -3721,17 +3675,13 @@
       <c r="J4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="5" t="s">
-        <v>40</v>
-      </c>
+      <c r="K4" s="5"/>
       <c r="L4" s="15" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
-      <c r="O4" s="5" t="s">
-        <v>42</v>
-      </c>
+      <c r="O4" s="5"/>
       <c r="P4" s="6" t="s">
         <v>31</v>
       </c>
@@ -3759,17 +3709,11 @@
       <c r="J5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="L5" s="12" t="s">
-        <v>41</v>
-      </c>
+      <c r="K5" s="5"/>
+      <c r="L5" s="12"/>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
-      <c r="O5" s="5" t="s">
-        <v>42</v>
-      </c>
+      <c r="O5" s="5"/>
       <c r="P5" s="6" t="s">
         <v>36</v>
       </c>
@@ -3782,7 +3726,7 @@
         <v>28</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>38</v>
@@ -3799,7 +3743,7 @@
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
       <c r="P6" s="6" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="15">
@@ -3810,7 +3754,7 @@
         <v>28</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>38</v>
@@ -3825,22 +3769,16 @@
       <c r="J7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="K7" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="L7" s="12" t="s">
-        <v>45</v>
-      </c>
+      <c r="K7" s="5"/>
+      <c r="L7" s="12"/>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
-      <c r="O7" s="5" t="s">
-        <v>42</v>
-      </c>
+      <c r="O7" s="5"/>
       <c r="P7" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="32">
+    <row r="8" spans="1:17" ht="15">
       <c r="A8" s="4" t="s">
         <v>27</v>
       </c>
@@ -3848,10 +3786,10 @@
         <v>28</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E8" s="4" t="b">
         <f>FALSE()</f>
@@ -3863,17 +3801,11 @@
       <c r="J8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="L8" s="15" t="s">
-        <v>67</v>
-      </c>
+      <c r="K8" s="5"/>
+      <c r="L8" s="15"/>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
-      <c r="O8" s="5" t="s">
-        <v>42</v>
-      </c>
+      <c r="O8" s="5"/>
       <c r="P8" s="6" t="s">
         <v>36</v>
       </c>
@@ -3886,10 +3818,10 @@
         <v>28</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E9" s="4" t="b">
         <f>FALSE()</f>
@@ -3906,7 +3838,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="32">
+    <row r="10" spans="1:17" ht="16">
       <c r="A10" s="4" t="s">
         <v>27</v>
       </c>
@@ -3914,10 +3846,10 @@
         <v>28</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E10" s="4" t="b">
         <f>FALSE()</f>
@@ -3929,17 +3861,13 @@
       <c r="J10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="K10" s="5" t="s">
-        <v>40</v>
-      </c>
+      <c r="K10" s="5"/>
       <c r="L10" s="15" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
-      <c r="O10" s="5" t="s">
-        <v>42</v>
-      </c>
+      <c r="O10" s="5"/>
       <c r="P10" s="6" t="s">
         <v>36</v>
       </c>
@@ -3952,10 +3880,10 @@
         <v>28</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E11" s="4" t="b">
         <f>FALSE()</f>
@@ -3968,7 +3896,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="12"/>
       <c r="M11" s="5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>

</xml_diff>

<commit_message>
term by lookup tweaks for refdata
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Death.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Death.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/work/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBDC7842-0A3A-714C-9128-63CE019AB624}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99DB18FA-8E30-6045-8E0D-345AFE55B533}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17200" yWindow="460" windowWidth="34400" windowHeight="28340" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17200" yWindow="460" windowWidth="34400" windowHeight="28340" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="notify_type_lookup" sheetId="11" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="73">
   <si>
     <t>casrec_code</t>
   </si>
@@ -257,6 +257,15 @@
   </si>
   <si>
     <t>proof_boolean_lookup</t>
+  </si>
+  <si>
+    <t>termby_lookup</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>O</t>
   </si>
 </sst>
 </file>
@@ -365,7 +374,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -394,6 +403,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2749,10 +2759,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:X1048576"/>
+  <dimension ref="A1:X10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -2794,16 +2804,305 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
+    <row r="2" spans="1:24" ht="15" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+    </row>
+    <row r="3" spans="1:24" ht="15">
+      <c r="A3" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+    </row>
+    <row r="4" spans="1:24" ht="15">
+      <c r="A4" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+    </row>
+    <row r="5" spans="1:24" ht="15">
+      <c r="E5" s="7"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+    </row>
+    <row r="6" spans="1:24" ht="15">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+    </row>
+    <row r="7" spans="1:24" ht="15">
+      <c r="E7" s="7"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+    </row>
+    <row r="8" spans="1:24" ht="15">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+    </row>
+    <row r="9" spans="1:24" ht="14">
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+    </row>
+    <row r="10" spans="1:24" ht="15" customHeight="1">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:X1048576"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <cols>
+    <col min="1" max="1025" width="14.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" ht="15" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+    </row>
     <row r="2" spans="1:24" ht="15">
       <c r="A2" s="4" t="s">
-        <v>63</v>
+        <v>4</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="5" t="s">
-        <v>67</v>
+        <v>5</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -2853,6 +3152,266 @@
       <c r="X3" s="2"/>
     </row>
     <row r="4" spans="1:24" ht="15">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+    </row>
+    <row r="5" spans="1:24" ht="15">
+      <c r="E5" s="7"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+    </row>
+    <row r="6" spans="1:24" ht="15">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+    </row>
+    <row r="7" spans="1:24" ht="15">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+    </row>
+    <row r="8" spans="1:24" ht="14">
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+    </row>
+    <row r="9" spans="1:24" ht="15" customHeight="1">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+    </row>
+    <row r="1048576" ht="15.75" customHeight="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:X1048576"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <cols>
+    <col min="1" max="1025" width="14.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" ht="15" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+    </row>
+    <row r="2" spans="1:24" ht="15">
+      <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+    </row>
+    <row r="3" spans="1:24" ht="15">
+      <c r="E3" s="7"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+    </row>
+    <row r="4" spans="1:24" ht="15">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
       <c r="E4" s="7"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -2901,6 +3460,10 @@
       <c r="X5" s="2"/>
     </row>
     <row r="6" spans="1:24" ht="15">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
       <c r="E6" s="7"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -3003,533 +3566,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:X1048576"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
-  <cols>
-    <col min="1" max="1025" width="14.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:24" ht="15" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-    </row>
-    <row r="2" spans="1:24" ht="15">
-      <c r="A2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
-    </row>
-    <row r="3" spans="1:24" ht="15">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
-    </row>
-    <row r="4" spans="1:24" ht="15">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
-      <c r="W4" s="2"/>
-      <c r="X4" s="2"/>
-    </row>
-    <row r="5" spans="1:24" ht="15">
-      <c r="E5" s="7"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
-      <c r="V5" s="2"/>
-      <c r="W5" s="2"/>
-      <c r="X5" s="2"/>
-    </row>
-    <row r="6" spans="1:24" ht="15">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
-      <c r="U6" s="2"/>
-      <c r="V6" s="2"/>
-      <c r="W6" s="2"/>
-      <c r="X6" s="2"/>
-    </row>
-    <row r="7" spans="1:24" ht="15">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
-      <c r="V7" s="2"/>
-      <c r="W7" s="2"/>
-      <c r="X7" s="2"/>
-    </row>
-    <row r="8" spans="1:24" ht="14">
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
-      <c r="U8" s="2"/>
-      <c r="V8" s="2"/>
-      <c r="W8" s="2"/>
-      <c r="X8" s="2"/>
-    </row>
-    <row r="9" spans="1:24" ht="15" customHeight="1">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
-      <c r="U9" s="2"/>
-      <c r="V9" s="2"/>
-      <c r="W9" s="2"/>
-      <c r="X9" s="2"/>
-    </row>
-    <row r="1048576" ht="15.75" customHeight="1"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:X1048576"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
-  <cols>
-    <col min="1" max="1025" width="14.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:24" ht="15" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-    </row>
-    <row r="2" spans="1:24" ht="15">
-      <c r="A2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
-    </row>
-    <row r="3" spans="1:24" ht="15">
-      <c r="E3" s="7"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
-    </row>
-    <row r="4" spans="1:24" ht="15">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
-      <c r="W4" s="2"/>
-      <c r="X4" s="2"/>
-    </row>
-    <row r="5" spans="1:24" ht="15">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
-      <c r="V5" s="2"/>
-      <c r="W5" s="2"/>
-      <c r="X5" s="2"/>
-    </row>
-    <row r="6" spans="1:24" ht="15">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
-      <c r="U6" s="2"/>
-      <c r="V6" s="2"/>
-      <c r="W6" s="2"/>
-      <c r="X6" s="2"/>
-    </row>
-    <row r="7" spans="1:24" ht="15">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
-      <c r="V7" s="2"/>
-      <c r="W7" s="2"/>
-      <c r="X7" s="2"/>
-    </row>
-    <row r="8" spans="1:24" ht="14">
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
-      <c r="U8" s="2"/>
-      <c r="V8" s="2"/>
-      <c r="W8" s="2"/>
-      <c r="X8" s="2"/>
-    </row>
-    <row r="9" spans="1:24" ht="15" customHeight="1">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
-      <c r="U9" s="2"/>
-      <c r="V9" s="2"/>
-      <c r="W9" s="2"/>
-      <c r="X9" s="2"/>
-    </row>
-    <row r="1048576" ht="15.75" customHeight="1"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L6" sqref="L6"/>
+      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -3778,7 +3821,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15">
+    <row r="8" spans="1:17" ht="16">
       <c r="A8" s="4" t="s">
         <v>27</v>
       </c>
@@ -3802,7 +3845,9 @@
         <v>7</v>
       </c>
       <c r="K8" s="5"/>
-      <c r="L8" s="15"/>
+      <c r="L8" s="15" t="s">
+        <v>70</v>
+      </c>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>

</xml_diff>

<commit_message>
fix a few problem mapping things
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Death.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Death.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/work/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61B0C24-B42D-6543-8D78-46711B88E9E1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEDBFBAF-B8FD-EB46-9C51-FF661C5811B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17200" yWindow="460" windowWidth="34400" windowHeight="28340" tabRatio="500" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17200" yWindow="460" windowWidth="34400" windowHeight="28340" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="notify_type_lookup" sheetId="11" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="72">
   <si>
     <t>casrec_code</t>
   </si>
@@ -2764,7 +2764,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -3555,9 +3555,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L10" sqref="L10"/>
+      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -3917,9 +3917,7 @@
         <f>FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H11" s="5" t="s">
-        <v>39</v>
-      </c>
+      <c r="H11" s="5"/>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
       <c r="L11" s="12"/>

</xml_diff>

<commit_message>
change column name to match the migration project
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Death.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Death.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/work/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86AC6AE2-EAA1-004E-BD24-A21CB6A6B6E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1506B7E9-CDA4-104E-AD18-67BAA36F2BC9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1440" yWindow="460" windowWidth="34400" windowHeight="21940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -287,9 +287,6 @@
     <t>source_table_additional_columns</t>
   </si>
   <si>
-    <t>client_death_notfications</t>
-  </si>
-  <si>
     <t>death</t>
   </si>
   <si>
@@ -302,18 +299,19 @@
     <t>Term Type = D</t>
   </si>
   <si>
-    <t>Term Type
-Case</t>
-  </si>
-  <si>
     <t>deputy_death_notifications</t>
   </si>
   <si>
     <t>Stat = 99</t>
   </si>
   <si>
-    <t>Stat
-Deputy No</t>
+    <t>client_death_notifications</t>
+  </si>
+  <si>
+    <t>Term Type,Case</t>
+  </si>
+  <si>
+    <t>Stat,Deputy No</t>
   </si>
 </sst>
 </file>
@@ -819,7 +817,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -851,46 +849,46 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="28">
-      <c r="A2" t="s">
+      <c r="A2" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="16" t="s">
         <v>79</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>80</v>
       </c>
       <c r="D2" t="s">
         <v>27</v>
       </c>
       <c r="E2" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="G2" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="G2" s="16" t="s">
-        <v>83</v>
-      </c>
       <c r="H2" s="18" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="28">
       <c r="A3" s="16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D3" t="s">
         <v>27</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F3" s="16" t="s">
         <v>66</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H3" s="18" t="s">
         <v>87</v>

</xml_diff>